<commit_message>
readme y casos de prueba
</commit_message>
<xml_diff>
--- a/Casos de prueba BibCircular.xlsx
+++ b/Casos de prueba BibCircular.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Curso Python\MisProyectosDjango\BibliotecaCircular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D7381C-888A-4FE7-9900-F3CAAE5E660C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F8055B-065E-4639-853B-77A27E1A6D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2976" yWindow="2628" windowWidth="19104" windowHeight="9612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -86,6 +86,45 @@
   </si>
   <si>
     <t>Boton buscar sin escribir nada o que no encuentre datos.</t>
+  </si>
+  <si>
+    <t>Registrar usuarios, loguin y logout</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si </t>
+  </si>
+  <si>
+    <t>Revisar que sin loguearse no acceda a carga de libros, modicacion ni eliminacino</t>
+  </si>
+  <si>
+    <t>Caso #4</t>
+  </si>
+  <si>
+    <t>Caso #5</t>
+  </si>
+  <si>
+    <t>Caso #6</t>
+  </si>
+  <si>
+    <t>Cargar comentario sobre un libro y que aparezca en el listado debajo del libro</t>
+  </si>
+  <si>
+    <t>Caso #7</t>
+  </si>
+  <si>
+    <t>Listado de libros reservados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reservar libro. Revisar que se envie un mail al lugar con copia al usuario. </t>
+  </si>
+  <si>
+    <t>Caso #8</t>
+  </si>
+  <si>
+    <t>Listado de libros disponibles, que no aparezcan los reservados</t>
   </si>
 </sst>
 </file>
@@ -422,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -434,8 +473,8 @@
     <col min="2" max="2" width="40.33203125" customWidth="1"/>
     <col min="3" max="3" width="48.44140625" customWidth="1"/>
     <col min="4" max="4" width="61.44140625" customWidth="1"/>
-    <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="29.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" hidden="1" customWidth="1"/>
     <col min="7" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -520,11 +559,13 @@
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="8">
-        <v>44651</v>
+        <v>45189</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -545,20 +586,22 @@
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
     </row>
-    <row r="8" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="8">
-        <v>44651</v>
+        <v>45192</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -579,18 +622,22 @@
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
     </row>
-    <row r="9" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8">
-        <v>44651</v>
+        <v>45192</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -611,8 +658,186 @@
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:26" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8">
+        <v>45192</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+    </row>
+    <row r="11" spans="1:26" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8">
+        <v>45194</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+    </row>
+    <row r="12" spans="1:26" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8">
+        <v>45194</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+    </row>
+    <row r="13" spans="1:26" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8">
+        <v>45194</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
+    </row>
+    <row r="14" spans="1:26" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8">
+        <v>45195</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+    </row>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1591,6 +1816,8 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>